<commit_message>
Add flexibility to update properties in runtime for different tests #94
</commit_message>
<xml_diff>
--- a/selcukes-excel-runner/src/test/resources/TestData.xlsx
+++ b/selcukes-excel-runner/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\selcukes-excel-runner\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E949A5-653D-415D-93E9-95AB98C603A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0459B4-1244-4E3D-8EE8-4454FE38BBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{8ED8C800-1088-4943-A8AD-3DF4EB6B3031}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8ED8C800-1088-4943-A8AD-3DF4EB6B3031}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840F594A-4955-4E66-BD69-F84C673EB0D5}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,6 +712,7 @@
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -836,7 +837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1200F9D5-93C0-4617-A842-EFDA4EEB3250}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -846,6 +847,7 @@
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Parse Excel as Map of Maps #165
</commit_message>
<xml_diff>
--- a/selcukes-excel-runner/src/test/resources/TestData.xlsx
+++ b/selcukes-excel-runner/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\selcukes-excel-runner\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0459B4-1244-4E3D-8EE8-4454FE38BBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85588458-56E6-49B1-AC26-5B7DF448BF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8ED8C800-1088-4943-A8AD-3DF4EB6B3031}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8ED8C800-1088-4943-A8AD-3DF4EB6B3031}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
   <si>
     <t>Screen</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>Yahoo::Yahoo Login</t>
+  </si>
+  <si>
+    <t>Yahoo::Yahoo Home</t>
+  </si>
+  <si>
+    <t>Yahoo Home</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840F594A-4955-4E66-BD69-F84C673EB0D5}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,6 +601,18 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -603,10 +621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6068E7A2-F303-4CB3-9D5D-18DC8BE390E6}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,6 +708,18 @@
         <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -835,10 +865,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1200F9D5-93C0-4617-A842-EFDA4EEB3250}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,6 +968,27 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>